<commit_message>
Se realizan algunos cambios en la importacion del excel y para mostrar los partidos jugados hasta la fecha actual.
</commit_message>
<xml_diff>
--- a/src/main/java/application/excel/BOCA.xlsx
+++ b/src/main/java/application/excel/BOCA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -38,9 +38,6 @@
     <t xml:space="preserve">isStudent</t>
   </si>
   <si>
-    <t xml:space="preserve">photo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Juan Roman</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t xml:space="preserve">true</t>
   </si>
   <si>
-    <t xml:space="preserve">https://media.minutouno.com/adjuntos/150/imagenes/028/851/0028851085.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Martin</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t xml:space="preserve">1991-08-25</t>
   </si>
   <si>
-    <t xml:space="preserve">https://as01.epimg.net/futbol/imagenes/2017/05/19/mas_futbol/1495188292_365499_1495188404_sumario_normal.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hugo</t>
   </si>
   <si>
@@ -77,9 +68,6 @@
     <t xml:space="preserve">1999-01-13</t>
   </si>
   <si>
-    <t xml:space="preserve">https://cdnmd.lavoz.com.ar/sites/default/files/styles/width_1072/public/deportes/nota_periodistica/iba_1.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Carlos</t>
   </si>
   <si>
@@ -89,9 +77,6 @@
     <t xml:space="preserve">1989-11-13</t>
   </si>
   <si>
-    <t xml:space="preserve">https://cdn.tn.com.ar/sites/default/files/styles/1366x765/public/2018/11/23/tevez-boca-camiseta.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fernando</t>
   </si>
   <si>
@@ -99,9 +84,6 @@
   </si>
   <si>
     <t xml:space="preserve">1979-11-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.infobae.com/new-resizer/pDhJOFP13eEFc6QtftoK0ZirKiY=/1200x0/filters:quality(100)/s3.amazonaws.com/arc-wordpress-client-uploads/infobae-wp/wp-content/uploads/2018/07/27123413/Fernando-Gago-triste.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre Equipo</t>
@@ -118,7 +100,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -143,13 +125,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -197,7 +172,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -207,10 +182,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -231,21 +202,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F65536"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,119 +233,94 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>12345678</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>12345679</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>12345677</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>19345677</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>19345677</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://media.minutouno.com/adjuntos/150/imagenes/028/851/0028851085.jpg"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://as01.epimg.net/futbol/imagenes/2017/05/19/mas_futbol/1495188292_365499_1495188404_sumario_normal.jpg"/>
-    <hyperlink ref="F4" r:id="rId3" display="https://cdnmd.lavoz.com.ar/sites/default/files/styles/width_1072/public/deportes/nota_periodistica/iba_1.jpg"/>
-    <hyperlink ref="F5" r:id="rId4" display="https://cdn.tn.com.ar/sites/default/files/styles/1366x765/public/2018/11/23/tevez-boca-camiseta.jpg"/>
-    <hyperlink ref="F6" r:id="rId5" display="https://www.infobae.com/new-resizer/pDhJOFP13eEFc6QtftoK0ZirKiY=/1200x0/filters:quality(100)/s3.amazonaws.com/arc-wordpress-client-uploads/infobae-wp/wp-content/uploads/2018/07/27123413/Fernando-Gago-triste.jpg"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -400,19 +344,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1"/>
     </row>

</xml_diff>